<commit_message>
Adding comments for different page objects
</commit_message>
<xml_diff>
--- a/src/main/java/testData/TestCases.xlsx
+++ b/src/main/java/testData/TestCases.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A567BF78-A042-4A35-8578-67C757519FA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB6B525-EE37-497F-BFE5-72B63C2F499E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="58">
   <si>
     <t>Module Name</t>
   </si>
@@ -151,9 +151,6 @@
     <t>1.Hit the URL.                                                      2.Hover over the "Sports" tab on the main navbar.                                                                              3.Move to the "View ALL" option under the "Men" section in the dropdown menu.                         4 .Wait for the products to load.                               5.Select  "Lowest price" fiter from the "Sort" dropdown menu.                                                       6.Wait for the products to load.                                   7.Again select the "Recomended" filter from the "Sort" dropdown menu.                                   8.Wait for the products to load.</t>
   </si>
   <si>
-    <t>validating_links_of_different_section()</t>
-  </si>
-  <si>
     <t>Validating if all the links under jeans tab are redirecting to correct page or not.</t>
   </si>
   <si>
@@ -161,13 +158,58 @@
   </si>
   <si>
     <t>validating_links_of_different_section</t>
+  </si>
+  <si>
+    <t>checking_filter</t>
+  </si>
+  <si>
+    <t>Validating number of products before and after selection of price filter</t>
+  </si>
+  <si>
+    <t>1. Hit the URL
+2. Hover on Skin and Select Face masks under Treatments 2nd Level Category
+3. In Category Listing Page, Select Price Range Filter Ex: "£15 - £30".
+4. Verify the Entire Results list displayed based on the Filtered Price Range
+5. Remove the filter and Verify Entire Original list of values are displayed</t>
+  </si>
+  <si>
+    <t>links_test</t>
+  </si>
+  <si>
+    <t>Validating the cart page after adding a product from the clothing section.</t>
+  </si>
+  <si>
+    <t>1. Hit the URL
+2. Click on Clothing in the category Section
+3. Add a product to cart with below conditions
+a. Add product with Max discounted price with 3 quantities.
+b. Add with available size.
+4. Navigate To Cart Page and Verify All the Details &amp; Calculations of the products should be same as details while adding to cart</t>
+  </si>
+  <si>
+    <t>registration_test</t>
+  </si>
+  <si>
+    <t>Entering values in different fields and registering a user.</t>
+  </si>
+  <si>
+    <t>validating_password</t>
+  </si>
+  <si>
+    <t>Validating generated password for different lengths.</t>
+  </si>
+  <si>
+    <t>1. Hit the URL                                                                                                    2. Navigate To Signup Screen                                                                       3. Enter All the Information either optional or Mandatory in the Form Until Password Field.                                                                       4. Click Generate Password                                                                              5. Verify System Can generate Password Less than 64 Characters only but not more.                                                                     6. Generate Password with 20 characters and enter them in Account Security Field.                          7. Verify Successfully registered after Clicking Register Button and Verify Entered values in Account Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Hit the URL                                                                                                    2. Navigate To Signup Screen                                                                       3. Enter All the Information either optional or Mandatory in the Form Until Password Field.                                                                       4. Click Generate Password                                                                              5. Verify System Can generate Password Less than 64 Characters only but not more.      6.Verify System Can generate Password Less than 8 Characters and more.                                                                     </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,6 +237,13 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -216,7 +265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -236,6 +285,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -517,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A98942-7FE4-49AD-84B2-87D3542DBE3B}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -722,29 +774,85 @@
     </row>
     <row r="14" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="B15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="145" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="174" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>4</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B19" t="s">
         <v>4</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C19" t="s">
         <v>4</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D19" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>